<commit_message>
add 3V3LDO & pad
</commit_message>
<xml_diff>
--- a/CAN_Dual_MDexpress-BOM.xlsx
+++ b/CAN_Dual_MDexpress-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUTO\OneDrive\Documents\KiCAD\H-Bridge-MD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{2EFBFD01-2460-4F3C-8BB2-B436FD855680}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{98BB7FBB-4BB9-4035-A7B5-F4D2B6A29628}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{2EFBFD01-2460-4F3C-8BB2-B436FD855680}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{9FE2463A-4CE1-40DA-AA19-6DD53B3BC1A7}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="14400" windowHeight="10065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN_Dual_MDexpress-BOM" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>SI8650AB-B-IS1</t>
   </si>
@@ -36,9 +36,6 @@
     <t>A3921KLPTR-T</t>
   </si>
   <si>
-    <t>NVMFD5C446NT1G</t>
-  </si>
-  <si>
     <t>GRM21BR71H104KA01L</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>ERJ-3RED21R0V</t>
   </si>
   <si>
-    <t>CRGCQ0603F2K2</t>
-  </si>
-  <si>
     <t>AZ2085D-ADJTRG1</t>
   </si>
   <si>
@@ -78,69 +72,12 @@
     <t>MCP2562-E/SN</t>
   </si>
   <si>
-    <t>PTS647SM38SMTR2LFS</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Wurth-Elektronik/150060RS75000?qs=sGAEpiMZZMseGfSY3csMkQ6oANueNQcIZZLd5sCt8%252BgHOxPA66eP1Q%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Wurth-Elektronik/150060VS75000?qs=sGAEpiMZZMseGfSY3csMkQ6oANueNQcILlzQzAXA7sDRB8sKt%252BAFmQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Comchip-Technology/CDBU0340?qs=sGAEpiMZZMtQ8nqTKtFS%2FLInc5CjRwvsMxlvxMjqWf8%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Silicon-Labs/SI8650AB-B-IS1?qs=sGAEpiMZZMssyD0wnx%2FymM3bPDptwQTOrws2oQSEEHP4PRc8a2RfbQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.digikey.jp/product-detail/ja/allegro-microsystems/A3921KLPTR-T/620-1523-1-ND/4318335</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/863-NVMFD5C446NT1G</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Vishay-Dale/CRCW060310K0JNEAC?qs=sGAEpiMZZMvdGkrng054t0DrEhLhGh8gI%252BMkPfXq1W4BiYWjDL9dTQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Yageo/RC0603FR-073KL?qs=sGAEpiMZZMvdGkrng054t8Tx25L%252BvTaR1yPw6j6EgfE%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Vishay-Dale/CRCW06033K74FKEA?qs=sGAEpiMZZMvdGkrng054tw79ugaueG8BIMJ8mgwbk90%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Panasonic/ERJ-3RBD1201V?qs=sGAEpiMZZMvdGkrng054t29VXh6xaPxCdEoyV4AjjwRIjvw2K%2Fv8Ew%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Panasonic/ERJ-3RED21R0V?qs=sGAEpiMZZMvdGkrng054t29VXh6xaPxCzrmsBJ0cGNBrLTCNmlFwhA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/TE-Connectivity-Holsworthy/CRGCQ0603F2K2?qs=sGAEpiMZZMvdGkrng054t7z4BkURc4Lz8GbtTKdku6X327MzAzVS9g%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Diodes-Incorporated/AZ2085D-ADJTRG1?qs=sGAEpiMZZMsGz1a6aV8DcOA9IcEEBBoKo0ds3qpDRyE%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/STMicroelectronics/STM32F042K6T6TR?qs=sGAEpiMZZMve4%2FbfQkoj%252BPGyMe7gbWABvdDz%252BMbHBeE%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/Microchip-Technology/MCP2562-E-SN?qs=sGAEpiMZZMsGqoCZrYwANiyhCBJiqvV6gstIhlvqgro%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.jp/ProductDetail/611-PTS647SM38SMTR2L</t>
-  </si>
-  <si>
     <t>C11,C17</t>
   </si>
   <si>
     <t>GCM21BR71H474KA55L</t>
   </si>
   <si>
-    <t>C1,C2,C3,C4,C5,C6,C8,C9,C10,C12,C14,C15,C16,C18</t>
-  </si>
-  <si>
-    <t>C7,C13</t>
-  </si>
-  <si>
     <t>150060RS75000</t>
   </si>
   <si>
@@ -159,9 +96,6 @@
     <t>Q1,Q2,Q3,Q4</t>
   </si>
   <si>
-    <t>R9,R10,R11,R30,R31,R32,R33</t>
-  </si>
-  <si>
     <t>R24,R27</t>
   </si>
   <si>
@@ -174,19 +108,10 @@
     <t>R4,R5,R12,R13,R16,R17,R20,R21</t>
   </si>
   <si>
-    <t>R1,R2,R3,R6</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
     <t>U3</t>
-  </si>
-  <si>
-    <t>SW1</t>
   </si>
   <si>
     <t>Designator</t>
@@ -205,8 +130,44 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>D3,D4,D5,D8,D9,D10,D11</t>
+    <t>C1,C3</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CL21B105KBFNNNE</t>
+  </si>
+  <si>
+    <t>D3,D4,D8,D9,D10,D11</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVMFD5C466NLT1G</t>
+  </si>
+  <si>
+    <t>R10,R30,R31,R32,R33</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RN1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXB-38V222JV</t>
+  </si>
+  <si>
+    <t>C4,C5,C6,C8,C9,C10,C12,C14,C15,C16,C18</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>U1,U4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>C2,C7,C13,C19</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.digikey.jp/product-detail/ja/allegro-microsystems/A3921KLPTR-T/620-1523-1-ND/4318335</t>
   </si>
 </sst>
 </file>
@@ -817,7 +778,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -835,6 +796,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1192,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -1206,280 +1173,250 @@
     <col min="4" max="4" width="152.77734375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="6">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>22</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>4</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="6">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6">
+        <v>16</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6">
+        <v>4</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2">
+      <c r="C19" s="7">
         <v>4</v>
       </c>
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>28</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C5">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="B20" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C20" s="7">
         <v>2</v>
       </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>32</v>
-      </c>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="2"/>
@@ -1490,16 +1427,6 @@
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>